<commit_message>
updated OrbitTradeSpace and added loop parameters for orbit design
</commit_message>
<xml_diff>
--- a/Space Mission Design and Navigation/Final Project/orbitData.xlsx
+++ b/Space Mission Design and Navigation/Final Project/orbitData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dillon's Laptop\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dillon's Laptop\Documents\GitHub\JHUCode\Space Mission Design and Navigation\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{930DCE0A-0C85-4E99-B834-AAA579283390}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C6615D-91AF-4E03-9384-03E973E26131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15330" yWindow="1650" windowWidth="21600" windowHeight="11385" xr2:uid="{D4D777B6-936A-4172-99CA-C3BF2E35C73C}"/>
+    <workbookView xWindow="5775" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{D4D777B6-936A-4172-99CA-C3BF2E35C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Sa</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Orbit3</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A5:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,27 +435,27 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>68.972200000000001</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>30.1111</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>3.3054999999999999</v>

</xml_diff>

<commit_message>
first orbit plot, cost, validation
First round of orbital data plotted and saved, cost functions programmed in, statistical validation started but not really understood...
</commit_message>
<xml_diff>
--- a/Space Mission Design and Navigation/Final Project/orbitData.xlsx
+++ b/Space Mission Design and Navigation/Final Project/orbitData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dillon's Laptop\Documents\GitHub\JHUCode\Space Mission Design and Navigation\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C6615D-91AF-4E03-9384-03E973E26131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26562EDA-D83A-488D-AA45-204E3EA5FA3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{D4D777B6-936A-4172-99CA-C3BF2E35C73C}"/>
+    <workbookView xWindow="5775" yWindow="1035" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{D4D777B6-936A-4172-99CA-C3BF2E35C73C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Orbit Tables" sheetId="1" r:id="rId1"/>
+    <sheet name="Orbit 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Ion</t>
   </si>
@@ -67,16 +68,28 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Orbit4</t>
+  </si>
+  <si>
+    <t>Ground Contacts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,6 +133,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>500516</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>178246</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{751F62BE-CE3D-4E06-9970-0756F278C6F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1666875" y="781049"/>
+          <a:ext cx="5367791" cy="2445197"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD216C4-95C9-4600-82D8-4578F9C7C6E4}">
-  <dimension ref="A5:I8"/>
+  <dimension ref="A5:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,19 +526,19 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>68.972200000000001</v>
+        <v>39.805599999999998</v>
       </c>
       <c r="C6">
-        <v>1.0278</v>
+        <v>0.77780000000000005</v>
       </c>
       <c r="D6" s="1">
-        <v>28378.15</v>
+        <v>28378</v>
       </c>
       <c r="E6">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="F6">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G6">
         <v>-90</v>
@@ -487,22 +555,22 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>30.1111</v>
+        <v>68.972200000000001</v>
       </c>
       <c r="C7">
-        <v>3.4722</v>
+        <v>1.0278</v>
       </c>
       <c r="D7" s="1">
-        <v>32378.15</v>
+        <v>28378.15</v>
       </c>
       <c r="E7">
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G7">
-        <v>-50</v>
+        <v>-90</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -516,31 +584,140 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>3.3054999999999999</v>
+        <v>30.1111</v>
       </c>
       <c r="C8">
-        <v>6.4165999999999999</v>
+        <v>3.4722</v>
       </c>
       <c r="D8" s="1">
         <v>32378.15</v>
       </c>
       <c r="E8">
+        <v>0.35</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <v>-50</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>3.3054999999999999</v>
+      </c>
+      <c r="C9">
+        <v>6.4165999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>32378.15</v>
+      </c>
+      <c r="E9">
         <v>0.75</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>71</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>-20</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB55498-12C2-4AAD-A936-51E25816E3C4}">
+  <dimension ref="B2:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E2:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>39.805599999999998</v>
+      </c>
+      <c r="D3">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <v>28378</v>
+      </c>
+      <c r="F3">
+        <v>0.6</v>
+      </c>
+      <c r="G3">
+        <v>75</v>
+      </c>
+      <c r="H3">
+        <v>-90</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>